<commit_message>
Ralationships of formation energy vs point defect formation energy
</commit_message>
<xml_diff>
--- a/final_metal_oxide_properties.xlsx
+++ b/final_metal_oxide_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saleheen\Desktop\materials_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2D65F-ADA8-4DC5-A5E9-142801961945}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1809E9B6-F15C-44B8-80FE-5FE9039E7064}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" activeTab="3" xr2:uid="{A4A5F5A1-0C63-45A1-9EB4-51F055D8EA08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" firstSheet="1" activeTab="7" xr2:uid="{A4A5F5A1-0C63-45A1-9EB4-51F055D8EA08}"/>
   </bookViews>
   <sheets>
     <sheet name="reduced_properties" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="oxide_pairs" sheetId="1" r:id="rId3"/>
     <sheet name="oxide_correlation" sheetId="4" r:id="rId4"/>
     <sheet name="bulk_vacancy" sheetId="5" r:id="rId5"/>
-    <sheet name="goxide_per_o_atom" sheetId="7" r:id="rId6"/>
+    <sheet name="goxide_mp" sheetId="7" r:id="rId6"/>
     <sheet name="surface_formation_energy" sheetId="6" r:id="rId7"/>
+    <sheet name="formation_energy_corr" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">oxide_pairs!$A$1:$X$298</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="620">
   <si>
     <t>Ac2O3</t>
   </si>
@@ -1472,9 +1473,6 @@
     <t>coo</t>
   </si>
   <si>
-    <t>eu2o3</t>
-  </si>
-  <si>
     <t>fe2o3</t>
   </si>
   <si>
@@ -1724,9 +1722,6 @@
     <t>https://doi.org/10.1021/acsami.7b06139</t>
   </si>
   <si>
-    <t>Comp</t>
-  </si>
-  <si>
     <t>100, 111</t>
   </si>
   <si>
@@ -1908,6 +1903,21 @@
   </si>
   <si>
     <t>formation_per_O</t>
+  </si>
+  <si>
+    <t>oxides</t>
+  </si>
+  <si>
+    <t>formation_energy_per_o_atom (eV)</t>
+  </si>
+  <si>
+    <t>surface_formation_energy( eV/Å2)</t>
+  </si>
+  <si>
+    <t>surface_vacancy_formation_energy (eV)</t>
+  </si>
+  <si>
+    <t>bulk_vacancy_formation_energy (eV)</t>
   </si>
 </sst>
 </file>
@@ -2227,7 +2237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2638,6 +2648,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2698,43 +2747,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -10241,73 +10260,73 @@
         <v>233</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="25" t="s">
         <v>498</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="32" t="s">
         <v>499</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>500</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>501</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="28" t="s">
         <v>502</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>503</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="K1" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>536</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="O1" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="M1" s="33" t="s">
-        <v>537</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="27" t="s">
         <v>512</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>513</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="X1" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="Y1" s="17" t="s">
         <v>516</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="Y1" s="17" t="s">
-        <v>517</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>350</v>
@@ -10365,7 +10384,7 @@
         <v>-11.473286003005649</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -10385,7 +10404,7 @@
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z2" s="2">
         <v>1977</v>
@@ -10459,7 +10478,7 @@
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z3" s="2">
         <v>200</v>
@@ -10481,7 +10500,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -10532,7 +10551,7 @@
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>304</v>
@@ -10554,7 +10573,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -10621,7 +10640,7 @@
         <v>5</v>
       </c>
       <c r="Y5" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z5" s="2" t="s">
         <v>304</v>
@@ -10643,7 +10662,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -10695,7 +10714,7 @@
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z6" s="2">
         <v>312</v>
@@ -10717,7 +10736,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -10769,7 +10788,7 @@
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z7" s="2">
         <v>315</v>
@@ -10791,7 +10810,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
@@ -10858,7 +10877,7 @@
         <v>5</v>
       </c>
       <c r="Y8" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z8" s="2">
         <v>150</v>
@@ -10880,7 +10899,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
@@ -10932,7 +10951,7 @@
       </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z9" s="2">
         <v>450</v>
@@ -10988,7 +11007,7 @@
         <v>5.4619889101932939</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -11008,7 +11027,7 @@
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z10" s="2">
         <v>2000</v>
@@ -11082,7 +11101,7 @@
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z11" s="2">
         <v>1972</v>
@@ -11156,7 +11175,7 @@
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z12" s="2">
         <v>450</v>
@@ -11230,7 +11249,7 @@
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z13" s="2">
         <v>2577</v>
@@ -11304,7 +11323,7 @@
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z14" s="2">
         <v>817</v>
@@ -11377,7 +11396,7 @@
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Z15" s="2" t="s">
         <v>304</v>
@@ -11450,7 +11469,7 @@
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z16" s="2">
         <v>305</v>
@@ -11524,7 +11543,7 @@
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z17" s="2">
         <v>2898</v>
@@ -11546,7 +11565,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>27</v>
@@ -11598,7 +11617,7 @@
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z18" s="2">
         <v>1430</v>
@@ -11671,7 +11690,7 @@
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Z19" s="2" t="s">
         <v>304</v>
@@ -11744,7 +11763,7 @@
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Z20" s="2" t="s">
         <v>304</v>
@@ -11818,7 +11837,7 @@
       </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z21" s="2">
         <v>2210</v>
@@ -11840,7 +11859,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>30</v>
@@ -11891,7 +11910,7 @@
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Z22" s="2" t="s">
         <v>304</v>
@@ -11913,7 +11932,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>33</v>
@@ -11964,7 +11983,7 @@
       </c>
       <c r="X23" s="2"/>
       <c r="Y23" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z23" s="2" t="s">
         <v>304</v>
@@ -11983,7 +12002,7 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>32</v>
@@ -12034,7 +12053,7 @@
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z24" s="2" t="s">
         <v>304</v>
@@ -12120,7 +12139,7 @@
         <v>1</v>
       </c>
       <c r="Y25" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z25" s="2">
         <v>2400</v>
@@ -12189,7 +12208,7 @@
       </c>
       <c r="X26" s="2"/>
       <c r="Y26" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z26" s="2">
         <v>900</v>
@@ -12273,7 +12292,7 @@
         <v>1</v>
       </c>
       <c r="Y27" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z27" s="2">
         <v>1830</v>
@@ -12341,7 +12360,7 @@
       </c>
       <c r="X28" s="2"/>
       <c r="Y28" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z28" s="2" t="s">
         <v>304</v>
@@ -12426,7 +12445,7 @@
         <v>3</v>
       </c>
       <c r="Y29" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z29" s="2">
         <v>2329</v>
@@ -12494,7 +12513,7 @@
       </c>
       <c r="X30" s="2"/>
       <c r="Y30" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z30" s="2">
         <v>300</v>
@@ -12700,7 +12719,7 @@
       </c>
       <c r="X33" s="2"/>
       <c r="Y33" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z33" s="2">
         <v>490</v>
@@ -12768,7 +12787,7 @@
       </c>
       <c r="X34" s="2"/>
       <c r="Y34" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z34" s="2">
         <v>590</v>
@@ -12836,7 +12855,7 @@
       </c>
       <c r="X35" s="2"/>
       <c r="Y35" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z35" s="2">
         <v>164</v>
@@ -12905,7 +12924,7 @@
       </c>
       <c r="X36" s="2"/>
       <c r="Y36" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z36" s="2">
         <v>432</v>
@@ -12974,7 +12993,7 @@
       </c>
       <c r="X37" s="2"/>
       <c r="Y37" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z37" s="2">
         <v>1235</v>
@@ -13042,7 +13061,7 @@
       </c>
       <c r="X38" s="2"/>
       <c r="Y38" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z38" s="2" t="s">
         <v>304</v>
@@ -13127,7 +13146,7 @@
         <v>6</v>
       </c>
       <c r="Y39" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z39" s="2">
         <v>1446</v>
@@ -13196,7 +13215,7 @@
       </c>
       <c r="X40" s="2"/>
       <c r="Y40" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z40" s="2">
         <v>2228</v>
@@ -13265,7 +13284,7 @@
       </c>
       <c r="X41" s="2"/>
       <c r="Y41" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z41" s="2">
         <v>2344</v>
@@ -13334,7 +13353,7 @@
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z42" s="2">
         <v>2291</v>
@@ -13402,7 +13421,7 @@
       </c>
       <c r="X43" s="2"/>
       <c r="Y43" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z43" s="2" t="s">
         <v>304</v>
@@ -13487,7 +13506,7 @@
         <v>3</v>
       </c>
       <c r="Y44" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z44" s="2">
         <v>1565</v>
@@ -13556,7 +13575,7 @@
       </c>
       <c r="X45" s="2"/>
       <c r="Y45" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z45" s="2">
         <v>1597</v>
@@ -13625,7 +13644,7 @@
       </c>
       <c r="X46" s="2"/>
       <c r="Y46" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z46" s="2">
         <v>1377</v>
@@ -13694,7 +13713,7 @@
       </c>
       <c r="X47" s="2"/>
       <c r="Y47" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z47" s="2">
         <v>1806</v>
@@ -13763,7 +13782,7 @@
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z48" s="2">
         <v>2339</v>
@@ -13832,7 +13851,7 @@
       </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z49" s="2">
         <v>1115</v>
@@ -13901,7 +13920,7 @@
       </c>
       <c r="X50" s="2"/>
       <c r="Y50" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z50" s="2">
         <v>2774</v>
@@ -13970,7 +13989,7 @@
       </c>
       <c r="X51" s="2"/>
       <c r="Y51" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z51" s="2">
         <v>500</v>
@@ -14039,7 +14058,7 @@
       </c>
       <c r="X52" s="2"/>
       <c r="Y52" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z52" s="2">
         <v>2330</v>
@@ -14107,7 +14126,7 @@
       </c>
       <c r="X53" s="2"/>
       <c r="Y53" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z53" s="2">
         <v>300</v>
@@ -14176,7 +14195,7 @@
       </c>
       <c r="X54" s="2"/>
       <c r="Y54" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z54" s="2">
         <v>1912</v>
@@ -14261,7 +14280,7 @@
         <v>4</v>
       </c>
       <c r="Y55" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z55" s="2">
         <v>1100</v>
@@ -14329,7 +14348,7 @@
       </c>
       <c r="X56" s="2"/>
       <c r="Y56" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z56" s="2" t="s">
         <v>304</v>
@@ -14398,7 +14417,7 @@
       </c>
       <c r="X57" s="2"/>
       <c r="Y57" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z57" s="2">
         <v>350</v>
@@ -14467,7 +14486,7 @@
       </c>
       <c r="X58" s="2"/>
       <c r="Y58" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z58" s="2">
         <v>490</v>
@@ -14536,7 +14555,7 @@
       </c>
       <c r="X59" s="2"/>
       <c r="Y59" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z59" s="2">
         <v>380</v>
@@ -14605,7 +14624,7 @@
       </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z60" s="2">
         <v>2304</v>
@@ -14674,7 +14693,7 @@
       </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z61" s="2">
         <v>1570</v>
@@ -14743,7 +14762,7 @@
       </c>
       <c r="X62" s="2"/>
       <c r="Y62" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z62" s="2">
         <v>195</v>
@@ -14812,7 +14831,7 @@
       </c>
       <c r="X63" s="2"/>
       <c r="Y63" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z63" s="2">
         <v>2427</v>
@@ -14897,7 +14916,7 @@
         <v>1</v>
       </c>
       <c r="Y64" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z64" s="2">
         <v>2825</v>
@@ -14966,7 +14985,7 @@
       </c>
       <c r="X65" s="2"/>
       <c r="Y65" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z65" s="2">
         <v>1080</v>
@@ -15051,7 +15070,7 @@
         <v>4</v>
       </c>
       <c r="Y66" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z66" s="2">
         <v>1567</v>
@@ -15120,7 +15139,7 @@
       </c>
       <c r="X67" s="2"/>
       <c r="Y67" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z67" s="2">
         <v>1839</v>
@@ -15189,7 +15208,7 @@
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z68" s="2">
         <v>535</v>
@@ -15257,7 +15276,7 @@
       </c>
       <c r="X69" s="2"/>
       <c r="Y69" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z69" s="2" t="s">
         <v>304</v>
@@ -15342,7 +15361,7 @@
         <v>6</v>
       </c>
       <c r="Y70" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z70" s="2">
         <v>1100</v>
@@ -15411,7 +15430,7 @@
       </c>
       <c r="X71" s="2"/>
       <c r="Y71" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z71" s="2">
         <v>801</v>
@@ -15480,7 +15499,7 @@
       </c>
       <c r="X72" s="2"/>
       <c r="Y72" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z72" s="2">
         <v>1132</v>
@@ -15549,7 +15568,7 @@
       </c>
       <c r="X73" s="2"/>
       <c r="Y73" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z73" s="2">
         <v>675</v>
@@ -15618,7 +15637,7 @@
       </c>
       <c r="X74" s="2"/>
       <c r="Y74" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z74" s="2">
         <v>552</v>
@@ -15703,7 +15722,7 @@
         <v>6</v>
       </c>
       <c r="Y75" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z75" s="2">
         <v>1512</v>
@@ -15841,7 +15860,7 @@
       </c>
       <c r="X77" s="2"/>
       <c r="Y77" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z77" s="2">
         <v>1901</v>
@@ -15910,7 +15929,7 @@
       </c>
       <c r="X78" s="2"/>
       <c r="Y78" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z78" s="2">
         <v>2233</v>
@@ -15978,7 +15997,7 @@
       </c>
       <c r="X79" s="2"/>
       <c r="Y79" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z79" s="2" t="s">
         <v>304</v>
@@ -16062,7 +16081,7 @@
         <v>1</v>
       </c>
       <c r="Y80" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z80" s="2">
         <v>1955</v>
@@ -16130,7 +16149,7 @@
       </c>
       <c r="X81" s="2"/>
       <c r="Y81" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z81" s="2">
         <v>2547</v>
@@ -16198,7 +16217,7 @@
       </c>
       <c r="X82" s="2"/>
       <c r="Y82" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z82" s="2" t="s">
         <v>304</v>
@@ -16267,7 +16286,7 @@
       </c>
       <c r="X83" s="2"/>
       <c r="Y83" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z83" s="2">
         <v>41</v>
@@ -16335,7 +16354,7 @@
       </c>
       <c r="X84" s="2"/>
       <c r="Y84" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z84" s="2">
         <v>562</v>
@@ -16403,7 +16422,7 @@
       </c>
       <c r="X85" s="2"/>
       <c r="Y85" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z85" s="2" t="s">
         <v>304</v>
@@ -16471,7 +16490,7 @@
       </c>
       <c r="X86" s="2"/>
       <c r="Y86" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z86" s="2" t="s">
         <v>304</v>
@@ -16540,7 +16559,7 @@
       </c>
       <c r="X87" s="2"/>
       <c r="Y87" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z87" s="2">
         <v>830</v>
@@ -16609,7 +16628,7 @@
       </c>
       <c r="X88" s="2"/>
       <c r="Y88" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z88" s="2">
         <v>897</v>
@@ -16678,7 +16697,7 @@
       </c>
       <c r="X89" s="2"/>
       <c r="Y89" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z89" s="2">
         <v>290</v>
@@ -16763,7 +16782,7 @@
         <v>4</v>
       </c>
       <c r="Y90" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z90" s="2">
         <v>750</v>
@@ -16831,7 +16850,7 @@
       </c>
       <c r="X91" s="2"/>
       <c r="Y91" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z91" s="2" t="s">
         <v>304</v>
@@ -16899,7 +16918,7 @@
       </c>
       <c r="X92" s="2"/>
       <c r="Y92" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z92" s="2" t="s">
         <v>304</v>
@@ -16968,7 +16987,7 @@
       </c>
       <c r="X93" s="2"/>
       <c r="Y93" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z93" s="2">
         <v>2183</v>
@@ -17036,7 +17055,7 @@
       </c>
       <c r="X94" s="2"/>
       <c r="Y94" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z94" s="2" t="s">
         <v>304</v>
@@ -17120,7 +17139,7 @@
         <v>3</v>
       </c>
       <c r="Y95" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z95" s="2">
         <v>450</v>
@@ -17188,7 +17207,7 @@
       </c>
       <c r="X96" s="2"/>
       <c r="Y96" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z96" s="2" t="s">
         <v>304</v>
@@ -17256,7 +17275,7 @@
       </c>
       <c r="X97" s="2"/>
       <c r="Y97" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z97" s="2">
         <v>2400</v>
@@ -17325,7 +17344,7 @@
       </c>
       <c r="X98" s="2"/>
       <c r="Y98" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z98" s="2">
         <v>400</v>
@@ -17394,7 +17413,7 @@
       </c>
       <c r="X99" s="2"/>
       <c r="Y99" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z99" s="2">
         <v>570</v>
@@ -17462,7 +17481,7 @@
       </c>
       <c r="X100" s="2"/>
       <c r="Y100" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z100" s="2" t="s">
         <v>304</v>
@@ -17531,7 +17550,7 @@
       </c>
       <c r="X101" s="2"/>
       <c r="Y101" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z101" s="2">
         <v>412</v>
@@ -17600,7 +17619,7 @@
       </c>
       <c r="X102" s="2"/>
       <c r="Y102" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z102" s="2">
         <v>297</v>
@@ -17668,7 +17687,7 @@
       </c>
       <c r="X103" s="2"/>
       <c r="Y103" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z103" s="2">
         <v>400</v>
@@ -17752,7 +17771,7 @@
         <v>4</v>
       </c>
       <c r="Y104" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z104" s="2" t="s">
         <v>304</v>
@@ -17836,7 +17855,7 @@
         <v>4</v>
       </c>
       <c r="Y105" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z105" s="2">
         <v>1200</v>
@@ -17905,7 +17924,7 @@
       </c>
       <c r="X106" s="2"/>
       <c r="Y106" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z106" s="2">
         <v>25.4</v>
@@ -17974,7 +17993,7 @@
       </c>
       <c r="X107" s="2"/>
       <c r="Y107" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z107" s="2">
         <v>656</v>
@@ -18043,7 +18062,7 @@
       </c>
       <c r="X108" s="2"/>
       <c r="Y108" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z108" s="2">
         <v>380</v>
@@ -18112,7 +18131,7 @@
       </c>
       <c r="X109" s="2"/>
       <c r="Y109" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z109" s="2" t="s">
         <v>304</v>
@@ -18181,7 +18200,7 @@
       </c>
       <c r="X110" s="2"/>
       <c r="Y110" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z110" s="2">
         <v>2485</v>
@@ -18249,7 +18268,7 @@
       </c>
       <c r="X111" s="2"/>
       <c r="Y111" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z111" s="2" t="s">
         <v>304</v>
@@ -18318,7 +18337,7 @@
       </c>
       <c r="X112" s="2"/>
       <c r="Y112" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z112" s="2">
         <v>340</v>
@@ -18387,7 +18406,7 @@
       </c>
       <c r="X113" s="2"/>
       <c r="Y113" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z113" s="2">
         <v>1722</v>
@@ -18456,7 +18475,7 @@
       </c>
       <c r="X114" s="2"/>
       <c r="Y114" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z114" s="2">
         <v>2269</v>
@@ -18524,7 +18543,7 @@
       </c>
       <c r="X115" s="2"/>
       <c r="Y115" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z115" s="2" t="s">
         <v>304</v>
@@ -18593,7 +18612,7 @@
       </c>
       <c r="X116" s="2"/>
       <c r="Y116" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z116" s="2">
         <v>1080</v>
@@ -18677,7 +18696,7 @@
         <v>4</v>
       </c>
       <c r="Y117" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z117" s="2">
         <v>1630</v>
@@ -18746,7 +18765,7 @@
       </c>
       <c r="X118" s="2"/>
       <c r="Y118" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z118" s="2">
         <v>2531</v>
@@ -18814,7 +18833,7 @@
       </c>
       <c r="X119" s="2"/>
       <c r="Y119" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z119" s="2">
         <v>215</v>
@@ -18883,7 +18902,7 @@
       </c>
       <c r="X120" s="2"/>
       <c r="Y120" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z120" s="2">
         <v>1784</v>
@@ -18952,7 +18971,7 @@
       </c>
       <c r="X121" s="2"/>
       <c r="Y121" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z121" s="2">
         <v>2303</v>
@@ -19020,7 +19039,7 @@
       </c>
       <c r="X122" s="2"/>
       <c r="Y122" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z122" s="2">
         <v>119.5</v>
@@ -19088,7 +19107,7 @@
       </c>
       <c r="X123" s="2"/>
       <c r="Y123" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z123" s="2" t="s">
         <v>304</v>
@@ -19156,7 +19175,7 @@
       </c>
       <c r="X124" s="2"/>
       <c r="Y124" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z124" s="2" t="s">
         <v>304</v>
@@ -19225,7 +19244,7 @@
       </c>
       <c r="X125" s="2"/>
       <c r="Y125" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z125" s="2">
         <v>733</v>
@@ -19293,7 +19312,7 @@
       </c>
       <c r="X126" s="2"/>
       <c r="Y126" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z126" s="2">
         <v>430</v>
@@ -19361,7 +19380,7 @@
       </c>
       <c r="X127" s="2"/>
       <c r="Y127" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z127" s="2">
         <v>3390</v>
@@ -19429,7 +19448,7 @@
       </c>
       <c r="X128" s="2"/>
       <c r="Y128" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z128" s="2" t="s">
         <v>304</v>
@@ -19498,7 +19517,7 @@
       </c>
       <c r="X129" s="2"/>
       <c r="Y129" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z129" s="2">
         <v>1842</v>
@@ -19566,7 +19585,7 @@
       </c>
       <c r="X130" s="2"/>
       <c r="Y130" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z130" s="2" t="s">
         <v>304</v>
@@ -19635,7 +19654,7 @@
       </c>
       <c r="X131" s="2"/>
       <c r="Y131" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z131" s="2">
         <v>1777</v>
@@ -19703,7 +19722,7 @@
       </c>
       <c r="X132" s="2"/>
       <c r="Y132" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z132" s="2" t="s">
         <v>304</v>
@@ -19772,7 +19791,7 @@
       </c>
       <c r="X133" s="2"/>
       <c r="Y133" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z133" s="2">
         <v>1750</v>
@@ -19857,7 +19876,7 @@
         <v>4</v>
       </c>
       <c r="Y134" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z134" s="2">
         <v>1843</v>
@@ -19926,7 +19945,7 @@
       </c>
       <c r="X135" s="2"/>
       <c r="Y135" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z135" s="2">
         <v>579</v>
@@ -19994,7 +20013,7 @@
       </c>
       <c r="X136" s="2"/>
       <c r="Y136" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z136" s="2">
         <v>834</v>
@@ -20062,7 +20081,7 @@
       </c>
       <c r="X137" s="2"/>
       <c r="Y137" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z137" s="2" t="s">
         <v>304</v>
@@ -20131,7 +20150,7 @@
       </c>
       <c r="X138" s="2"/>
       <c r="Y138" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z138" s="2">
         <v>2341</v>
@@ -20200,7 +20219,7 @@
       </c>
       <c r="X139" s="2"/>
       <c r="Y139" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z139" s="2">
         <v>1300</v>
@@ -20269,7 +20288,7 @@
       </c>
       <c r="X140" s="2"/>
       <c r="Y140" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z140" s="2">
         <v>2827</v>
@@ -20338,7 +20357,7 @@
       </c>
       <c r="X141" s="2"/>
       <c r="Y141" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z141" s="2" t="s">
         <v>304</v>
@@ -20423,7 +20442,7 @@
         <v>3</v>
       </c>
       <c r="Y142" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z142" s="2">
         <v>2067</v>
@@ -20492,7 +20511,7 @@
       </c>
       <c r="X143" s="2"/>
       <c r="Y143" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z143" s="2">
         <v>670</v>
@@ -20561,7 +20580,7 @@
       </c>
       <c r="X144" s="2"/>
       <c r="Y144" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z144" s="2" t="s">
         <v>304</v>
@@ -20629,7 +20648,7 @@
       </c>
       <c r="X145" s="2"/>
       <c r="Y145" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z145" s="2" t="s">
         <v>304</v>
@@ -20697,7 +20716,7 @@
       </c>
       <c r="X146" s="2"/>
       <c r="Y146" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z146" s="2">
         <v>1967</v>
@@ -20765,7 +20784,7 @@
       </c>
       <c r="X147" s="2"/>
       <c r="Y147" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z147" s="2" t="s">
         <v>304</v>
@@ -20834,7 +20853,7 @@
       </c>
       <c r="X148" s="2"/>
       <c r="Y148" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z148" s="2">
         <v>1500</v>
@@ -20903,7 +20922,7 @@
       </c>
       <c r="X149" s="2"/>
       <c r="Y149" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z149" s="2">
         <v>1472</v>
@@ -20988,7 +21007,7 @@
         <v>1</v>
       </c>
       <c r="Y150" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z150" s="2">
         <v>2438</v>
@@ -21056,7 +21075,7 @@
       </c>
       <c r="X151" s="2"/>
       <c r="Y151" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z151" s="2" t="s">
         <v>304</v>
@@ -21141,7 +21160,7 @@
         <v>2</v>
       </c>
       <c r="Y152" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z152" s="2">
         <v>1974</v>
@@ -21201,7 +21220,7 @@
       </c>
       <c r="X153" s="2"/>
       <c r="Y153" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z153" s="2" t="s">
         <v>304</v>
@@ -21278,7 +21297,7 @@
         <v>6</v>
       </c>
       <c r="Y154" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z154" s="2">
         <v>2709</v>
@@ -35597,7 +35616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B73BE9-3FFE-475D-A723-92CE87E67446}">
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -35640,7 +35659,7 @@
         <v>350</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>459</v>
@@ -38767,10 +38786,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5644F9-DFD0-4528-8865-285E45E0996E}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38787,7 +38806,7 @@
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>459</v>
       </c>
@@ -38807,16 +38826,13 @@
         <v>465</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>460</v>
       </c>
@@ -38841,10 +38857,10 @@
         <v>337</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>466</v>
       </c>
@@ -38859,7 +38875,7 @@
         <v>2.863306617405442</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>467</v>
       </c>
@@ -38874,7 +38890,7 @@
         <v>3.0348957405408328E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>468</v>
       </c>
@@ -38889,13 +38905,10 @@
         <v>3.151560317405437</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>469</v>
       </c>
@@ -38910,13 +38923,13 @@
         <v>2.1207167974054499</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H6" s="39" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>470</v>
       </c>
@@ -38931,172 +38944,188 @@
         <v>3.8805203374054358</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>-198.95805204999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-190.60804726000001</v>
+      </c>
+      <c r="E8" s="2">
+        <f>D8+$F$2-C8</f>
+        <v>3.4207135174054315</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>561</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>472</v>
       </c>
       <c r="C9" s="2">
-        <v>-198.95805204999999</v>
+        <v>-370.91003302000001</v>
       </c>
       <c r="D9" s="2">
-        <v>-190.60804726000001</v>
+        <v>-363.25697377</v>
       </c>
       <c r="E9" s="2">
         <f>D9+$F$2-C9</f>
-        <v>3.4207135174054315</v>
+        <v>2.72376797740543</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>563</v>
-      </c>
-      <c r="H9" s="37" t="s">
+        <v>562</v>
+      </c>
+      <c r="H9" s="36" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>473</v>
       </c>
       <c r="C10" s="2">
-        <v>-370.91003302000001</v>
+        <v>-26.170262690000001</v>
       </c>
       <c r="D10" s="2">
-        <v>-363.25697377</v>
+        <v>-16.86637743</v>
       </c>
       <c r="E10" s="2">
         <f>D10+$F$2-C10</f>
-        <v>2.72376797740543</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>564</v>
-      </c>
-      <c r="H10" s="36" t="s">
+        <v>4.37459398740544</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>563</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>474</v>
       </c>
       <c r="C11" s="2">
-        <v>-26.170262690000001</v>
+        <v>-38.468832970000001</v>
       </c>
       <c r="D11" s="2">
-        <v>-16.86637743</v>
+        <v>-30.376762379999999</v>
       </c>
       <c r="E11" s="2">
         <f>D11+$F$2-C11</f>
-        <v>4.37459398740544</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>565</v>
-      </c>
-      <c r="H11" s="39" t="s">
+        <v>3.1627793174054446</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="H11" s="40" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="C12" s="2">
-        <v>-38.468832970000001</v>
-      </c>
-      <c r="D12" s="2">
-        <v>-30.376762379999999</v>
-      </c>
-      <c r="E12" s="2">
-        <f>D12+$F$2-C12</f>
-        <v>3.1627793174054446</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="H12" s="40" t="s">
+        <v>554</v>
+      </c>
+      <c r="H12" s="38" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="H13" s="38" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <v>-599.97843897999996</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-592.86837573000003</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" ref="E13:E30" si="1">D13+$F$2-C13</f>
+        <v>2.1807719774053567</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>477</v>
       </c>
       <c r="C14" s="2">
-        <v>-599.97843897999996</v>
+        <v>-211.90299375000001</v>
       </c>
       <c r="D14" s="2">
-        <v>-592.86837573000003</v>
+        <v>-204.22567572</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" ref="E14:E31" si="1">D14+$F$2-C14</f>
-        <v>2.1807719774053567</v>
+        <f t="shared" si="1"/>
+        <v>2.7480267574054551</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>567</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>478</v>
       </c>
       <c r="C15" s="2">
-        <v>-211.90299375000001</v>
+        <v>-62.134829379999999</v>
       </c>
       <c r="D15" s="2">
-        <v>-204.22567572</v>
+        <v>-52.416623219999998</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>2.7480267574054551</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>568</v>
+        <v>4.7889148874054399</v>
+      </c>
+      <c r="G15" s="2">
+        <v>100</v>
       </c>
       <c r="H15" s="39" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>479</v>
       </c>
       <c r="C16" s="2">
-        <v>-62.134829379999999</v>
+        <v>-89.201065069999999</v>
       </c>
       <c r="D16" s="2">
-        <v>-52.416623219999998</v>
+        <v>-79.460188040000006</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>4.7889148874054399</v>
-      </c>
-      <c r="G16" s="2">
-        <v>100</v>
-      </c>
-      <c r="H16" s="39" t="s">
+        <v>4.8115857574054388</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>567</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>549</v>
       </c>
     </row>
@@ -39105,41 +39134,41 @@
         <v>480</v>
       </c>
       <c r="C17" s="2">
-        <v>-89.201065069999999</v>
+        <v>-228.46961936</v>
       </c>
       <c r="D17" s="2">
-        <v>-79.460188040000006</v>
+        <v>-220.47352824000001</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>4.8115857574054388</v>
+        <v>3.0667998474054343</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>569</v>
+        <v>337</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>481</v>
       </c>
       <c r="C18" s="2">
-        <v>-228.46961936</v>
+        <v>-151.22276837999999</v>
       </c>
       <c r="D18" s="2">
-        <v>-220.47352824000001</v>
+        <v>-144.0289775</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>3.0667998474054343</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>551</v>
+        <v>2.2644996074054404</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -39147,20 +39176,14 @@
         <v>482</v>
       </c>
       <c r="C19" s="2">
-        <v>-151.22276837999999</v>
+        <v>-21.506446919999998</v>
       </c>
       <c r="D19" s="2">
-        <v>-144.0289775</v>
+        <v>-13.614792120000001</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>2.2644996074054404</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="H19" s="39" t="s">
-        <v>557</v>
+        <v>2.9623635274054365</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -39168,14 +39191,14 @@
         <v>483</v>
       </c>
       <c r="C20" s="2">
-        <v>-21.506446919999998</v>
+        <v>-119.22725527</v>
       </c>
       <c r="D20" s="2">
-        <v>-13.614792120000001</v>
+        <v>-110.98209944</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>2.9623635274054365</v>
+        <v>3.3158645574054475</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -39183,14 +39206,14 @@
         <v>484</v>
       </c>
       <c r="C21" s="2">
-        <v>-119.22725527</v>
+        <v>-145.1925918</v>
       </c>
       <c r="D21" s="2">
-        <v>-110.98209944</v>
+        <v>-137.94298309999999</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
-        <v>3.3158645574054475</v>
+        <v>2.3203174274054561</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -39198,14 +39221,14 @@
         <v>485</v>
       </c>
       <c r="C22" s="2">
-        <v>-145.1925918</v>
+        <v>-128.28174139999999</v>
       </c>
       <c r="D22" s="2">
-        <v>-137.94298309999999</v>
+        <v>-119.53463073</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
-        <v>2.3203174274054561</v>
+        <v>3.8178193974054295</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -39213,14 +39236,14 @@
         <v>486</v>
       </c>
       <c r="C23" s="2">
-        <v>-128.28174139999999</v>
+        <v>-22.725284030000001</v>
       </c>
       <c r="D23" s="2">
-        <v>-119.53463073</v>
+        <v>-14.542637109999999</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="1"/>
-        <v>3.8178193974054295</v>
+        <v>3.2533556474054421</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -39228,14 +39251,20 @@
         <v>487</v>
       </c>
       <c r="C24" s="2">
-        <v>-22.725284030000001</v>
+        <v>-37.303320249999999</v>
       </c>
       <c r="D24" s="2">
-        <v>-14.542637109999999</v>
+        <v>-29.109387139999999</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
-        <v>3.2533556474054421</v>
+        <v>3.264641837405442</v>
+      </c>
+      <c r="G24" s="2">
+        <v>110</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -39243,20 +39272,17 @@
         <v>488</v>
       </c>
       <c r="C25" s="2">
-        <v>-37.303320249999999</v>
+        <v>-129.09829221999999</v>
       </c>
       <c r="D25" s="2">
-        <v>-29.109387139999999</v>
+        <v>-121.46597087000001</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
-        <v>3.264641837405442</v>
-      </c>
-      <c r="G25" s="2">
-        <v>110</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>552</v>
+        <v>2.7030300774054297</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -39264,17 +39290,20 @@
         <v>489</v>
       </c>
       <c r="C26" s="2">
-        <v>-129.09829221999999</v>
+        <v>-104.14184631000001</v>
       </c>
       <c r="D26" s="2">
-        <v>-121.46597087000001</v>
+        <v>-97.75657047</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
-        <v>2.7030300774054297</v>
-      </c>
-      <c r="H26" s="42" t="s">
-        <v>570</v>
+        <v>1.4559845674054515</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -39282,20 +39311,14 @@
         <v>490</v>
       </c>
       <c r="C27" s="2">
-        <v>-104.14184631000001</v>
+        <v>-252.80621321000001</v>
       </c>
       <c r="D27" s="2">
-        <v>-97.75657047</v>
+        <v>-243.26874002</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
-        <v>1.4559845674054515</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>553</v>
+        <v>4.6081819174054601</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -39303,14 +39326,14 @@
         <v>491</v>
       </c>
       <c r="C28" s="2">
-        <v>-252.80621321000001</v>
+        <v>-452.11876445000001</v>
       </c>
       <c r="D28" s="2">
-        <v>-243.26874002</v>
+        <v>-444.95806028999999</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
-        <v>4.6081819174054601</v>
+        <v>2.2314128874054404</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -39318,14 +39341,14 @@
         <v>492</v>
       </c>
       <c r="C29" s="2">
-        <v>-452.11876445000001</v>
+        <v>-91.867609689999995</v>
       </c>
       <c r="D29" s="2">
-        <v>-444.95806028999999</v>
+        <v>-81.526373460000002</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
-        <v>2.2314128874054404</v>
+        <v>5.4119449574054386</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -39333,54 +39356,39 @@
         <v>493</v>
       </c>
       <c r="C30" s="2">
-        <v>-91.867609689999995</v>
+        <v>-241.15803285000001</v>
       </c>
       <c r="D30" s="2">
-        <v>-81.526373460000002</v>
+        <v>-231.75466761000001</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
-        <v>5.4119449574054386</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="C31" s="2">
-        <v>-241.15803285000001</v>
-      </c>
-      <c r="D31" s="2">
-        <v>-231.75466761000001</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" si="1"/>
         <v>4.4740739674054453</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="H31" s="40" t="s">
-        <v>554</v>
+      <c r="H30" s="40" t="s">
+        <v>553</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{6CDAE7FB-2E02-4C05-A982-CA04466BC29B}"/>
     <hyperlink ref="H6" r:id="rId2" xr:uid="{06F31AE8-331F-4702-B515-3117DD661AAD}"/>
-    <hyperlink ref="H9" r:id="rId3" display="https://doi.org/10.1088/1361-648X/aac743," xr:uid="{96B8D3C6-82CD-4DF7-A286-82FE6E4B6F0C}"/>
-    <hyperlink ref="H11" r:id="rId4" xr:uid="{DD30A351-E6D7-43CE-89F7-86CACDF97AE5}"/>
-    <hyperlink ref="H12" r:id="rId5" xr:uid="{39B8DCB9-A949-40A8-AB86-37835E33987A}"/>
-    <hyperlink ref="H13" r:id="rId6" tooltip="DOI URL" display="https://doi.org/10.1021/jp3004773" xr:uid="{62069577-4BEB-4A79-B7D4-C29E8BE881EE}"/>
-    <hyperlink ref="H31" r:id="rId7" xr:uid="{97CC427D-3951-4F87-9E91-B1DA106D14EF}"/>
-    <hyperlink ref="H15" r:id="rId8" xr:uid="{62482901-86CF-4ABE-B9F4-AC6AF73A8C42}"/>
-    <hyperlink ref="H16" r:id="rId9" xr:uid="{F3E23C30-6AD9-4049-ACD7-FCDD15052FC4}"/>
-    <hyperlink ref="H19" r:id="rId10" xr:uid="{2ECB89D4-DFD8-4AC4-9A36-E2928B476D6C}"/>
+    <hyperlink ref="H8" r:id="rId3" display="https://doi.org/10.1088/1361-648X/aac743," xr:uid="{96B8D3C6-82CD-4DF7-A286-82FE6E4B6F0C}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{DD30A351-E6D7-43CE-89F7-86CACDF97AE5}"/>
+    <hyperlink ref="H11" r:id="rId5" xr:uid="{39B8DCB9-A949-40A8-AB86-37835E33987A}"/>
+    <hyperlink ref="H12" r:id="rId6" tooltip="DOI URL" display="https://doi.org/10.1021/jp3004773" xr:uid="{62069577-4BEB-4A79-B7D4-C29E8BE881EE}"/>
+    <hyperlink ref="H30" r:id="rId7" xr:uid="{97CC427D-3951-4F87-9E91-B1DA106D14EF}"/>
+    <hyperlink ref="H14" r:id="rId8" xr:uid="{62482901-86CF-4ABE-B9F4-AC6AF73A8C42}"/>
+    <hyperlink ref="H15" r:id="rId9" xr:uid="{F3E23C30-6AD9-4049-ACD7-FCDD15052FC4}"/>
+    <hyperlink ref="H18" r:id="rId10" xr:uid="{2ECB89D4-DFD8-4AC4-9A36-E2928B476D6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
   <ignoredErrors>
-    <ignoredError sqref="G2 G18 G27 G31" numberStoredAsText="1"/>
+    <ignoredError sqref="G2 G17 G26 G30" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -39390,7 +39398,7 @@
   <dimension ref="A1:O298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39411,46 +39419,46 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>605</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>606</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>328</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>606</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="I1" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="32" t="s">
         <v>610</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="32" t="s">
         <v>611</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>612</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>613</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>614</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>615</v>
-      </c>
-      <c r="O1" s="32" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -47377,8 +47385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6790254-5CEC-4CFA-8812-D61E5E995C32}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47396,56 +47404,56 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>570</v>
+      </c>
+      <c r="C1" s="53" t="s">
         <v>571</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>572</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>573</v>
-      </c>
       <c r="D1" s="100" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="142" t="s">
         <v>460</v>
       </c>
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="144" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="164">
+      <c r="C2" s="146">
         <v>3.3904109706261301E-2</v>
       </c>
       <c r="D2" s="127">
         <v>3.0308439874054298</v>
       </c>
-      <c r="E2" s="142" t="s">
+      <c r="E2" s="155" t="s">
         <v>326</v>
       </c>
-      <c r="F2" s="169" t="s">
-        <v>597</v>
+      <c r="F2" s="138" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="161"/>
-      <c r="B3" s="163"/>
-      <c r="C3" s="165"/>
+      <c r="A3" s="143"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="147"/>
       <c r="D3" s="129">
         <v>3.3239820074054398</v>
       </c>
-      <c r="E3" s="143"/>
-      <c r="F3" s="169"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="138"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="142" t="s">
         <v>468</v>
       </c>
       <c r="B4" s="125">
@@ -47457,17 +47465,17 @@
       <c r="D4" s="130">
         <v>1.91862856740539</v>
       </c>
-      <c r="E4" s="142" t="s">
+      <c r="E4" s="155" t="s">
         <v>326</v>
       </c>
-      <c r="F4" s="169" t="s">
-        <v>596</v>
+      <c r="F4" s="138" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="166"/>
+      <c r="A5" s="148"/>
       <c r="B5" s="131" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C5" s="132">
         <v>0.32205517697242098</v>
@@ -47475,13 +47483,13 @@
       <c r="D5" s="133">
         <v>2.5098057874054498</v>
       </c>
-      <c r="E5" s="144"/>
-      <c r="F5" s="169"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="138"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="161"/>
+      <c r="A6" s="143"/>
       <c r="B6" s="111" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C6" s="112">
         <v>0.269542600903181</v>
@@ -47489,15 +47497,15 @@
       <c r="D6" s="129">
         <v>-1.12009968259455</v>
       </c>
-      <c r="E6" s="143"/>
-      <c r="F6" s="169"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="138"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="167" t="s">
+      <c r="A7" s="149" t="s">
         <v>469</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C7" s="55">
         <v>5.5445421405581598E-2</v>
@@ -47505,15 +47513,15 @@
       <c r="D7" s="56">
         <v>2.3577677274054101</v>
       </c>
-      <c r="E7" s="145" t="s">
-        <v>603</v>
-      </c>
-      <c r="F7" s="169"/>
+      <c r="E7" s="158" t="s">
+        <v>601</v>
+      </c>
+      <c r="F7" s="138"/>
     </row>
     <row r="8" spans="1:6" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="168"/>
+      <c r="A8" s="150"/>
       <c r="B8" s="57" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C8" s="58">
         <v>0.244539410765303</v>
@@ -47521,11 +47529,11 @@
       <c r="D8" s="59">
         <v>-3.8362542594540999E-2</v>
       </c>
-      <c r="E8" s="146"/>
-      <c r="F8" s="169"/>
+      <c r="E8" s="159"/>
+      <c r="F8" s="138"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="138" t="s">
+      <c r="A9" s="151" t="s">
         <v>470</v>
       </c>
       <c r="B9" s="125">
@@ -47537,15 +47545,15 @@
       <c r="D9" s="127">
         <v>0.57635066740544905</v>
       </c>
-      <c r="E9" s="147" t="s">
+      <c r="E9" s="160" t="s">
         <v>327</v>
       </c>
-      <c r="F9" s="169"/>
+      <c r="F9" s="138"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
+      <c r="A10" s="165"/>
       <c r="B10" s="48" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C10" s="49">
         <v>0.57080615585029004</v>
@@ -47553,13 +47561,13 @@
       <c r="D10" s="62">
         <v>1.83464093740545</v>
       </c>
-      <c r="E10" s="148"/>
-      <c r="F10" s="169"/>
+      <c r="E10" s="161"/>
+      <c r="F10" s="138"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="139"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="63" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C11" s="64">
         <v>0.15876409968765501</v>
@@ -47567,15 +47575,15 @@
       <c r="D11" s="65">
         <v>-0.54624473259457296</v>
       </c>
-      <c r="E11" s="149"/>
-      <c r="F11" s="169"/>
+      <c r="E11" s="162"/>
+      <c r="F11" s="138"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="153" t="s">
-        <v>472</v>
+      <c r="A12" s="166" t="s">
+        <v>471</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C12" s="55">
         <v>0.23859638425782301</v>
@@ -47583,15 +47591,15 @@
       <c r="D12" s="67">
         <v>4.0221599874054101</v>
       </c>
-      <c r="E12" s="147" t="s">
+      <c r="E12" s="160" t="s">
         <v>327</v>
       </c>
-      <c r="F12" s="170"/>
+      <c r="F12" s="139"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="154"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="71" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C13" s="50">
         <v>0.37717382066015598</v>
@@ -47599,15 +47607,15 @@
       <c r="D13" s="72">
         <v>-3.2670075425946798</v>
       </c>
-      <c r="E13" s="149"/>
-      <c r="F13" s="170"/>
+      <c r="E13" s="162"/>
+      <c r="F13" s="139"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="155" t="s">
-        <v>473</v>
+      <c r="A14" s="168" t="s">
+        <v>472</v>
       </c>
       <c r="B14" s="114" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C14" s="115">
         <v>0.15602959110056999</v>
@@ -47615,15 +47623,15 @@
       <c r="D14" s="116">
         <v>1.6800129474054299</v>
       </c>
-      <c r="E14" s="147" t="s">
+      <c r="E14" s="160" t="s">
         <v>327</v>
       </c>
-      <c r="F14" s="170"/>
+      <c r="F14" s="139"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="156"/>
+      <c r="A15" s="169"/>
       <c r="B15" s="111" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C15" s="112">
         <v>0.136699803612056</v>
@@ -47631,12 +47639,12 @@
       <c r="D15" s="113">
         <v>1.8519125174054201</v>
       </c>
-      <c r="E15" s="149"/>
-      <c r="F15" s="170"/>
+      <c r="E15" s="162"/>
+      <c r="F15" s="139"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="140" t="s">
-        <v>474</v>
+      <c r="A16" s="153" t="s">
+        <v>473</v>
       </c>
       <c r="B16" s="54">
         <v>110</v>
@@ -47647,15 +47655,15 @@
       <c r="D16" s="56">
         <v>3.6845018674054302</v>
       </c>
-      <c r="E16" s="147" t="s">
+      <c r="E16" s="160" t="s">
         <v>327</v>
       </c>
-      <c r="F16" s="169"/>
+      <c r="F16" s="138"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="157"/>
+      <c r="A17" s="170"/>
       <c r="B17" s="48" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C17" s="49">
         <v>0.560067840147913</v>
@@ -47663,13 +47671,13 @@
       <c r="D17" s="62" t="s">
         <v>304</v>
       </c>
-      <c r="E17" s="148"/>
-      <c r="F17" s="169"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="138"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="141"/>
+      <c r="A18" s="154"/>
       <c r="B18" s="73" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C18" s="74">
         <v>-6.5601907175453396E-3</v>
@@ -47677,15 +47685,15 @@
       <c r="D18" s="75">
         <v>2.5016611374053901</v>
       </c>
-      <c r="E18" s="149"/>
-      <c r="F18" s="169"/>
+      <c r="E18" s="162"/>
+      <c r="F18" s="138"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B19" s="121" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C19" s="122">
         <v>0.124803014354723</v>
@@ -47697,12 +47705,12 @@
         <v>326</v>
       </c>
       <c r="F19" s="97" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="158" t="s">
-        <v>476</v>
+      <c r="A20" s="140" t="s">
+        <v>475</v>
       </c>
       <c r="B20" s="54">
         <v>100</v>
@@ -47713,13 +47721,13 @@
       <c r="D20" s="56">
         <v>2.5408861074054099</v>
       </c>
-      <c r="E20" s="150" t="s">
+      <c r="E20" s="163" t="s">
         <v>327</v>
       </c>
-      <c r="F20" s="169"/>
+      <c r="F20" s="138"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="159"/>
+      <c r="A21" s="141"/>
       <c r="B21" s="117">
         <v>111</v>
       </c>
@@ -47729,12 +47737,12 @@
       <c r="D21" s="119">
         <v>2.1188442974054098</v>
       </c>
-      <c r="E21" s="151"/>
-      <c r="F21" s="169"/>
+      <c r="E21" s="164"/>
+      <c r="F21" s="138"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="78" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B22" s="79" t="s">
         <v>339</v>
@@ -47751,11 +47759,11 @@
       <c r="F22" s="98"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="138" t="s">
-        <v>478</v>
+      <c r="A23" s="151" t="s">
+        <v>477</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C23" s="60">
         <v>0.14058912840377499</v>
@@ -47763,15 +47771,15 @@
       <c r="D23" s="61">
         <v>1.51702027740543</v>
       </c>
-      <c r="E23" s="150" t="s">
+      <c r="E23" s="163" t="s">
         <v>327</v>
       </c>
-      <c r="F23" s="170"/>
+      <c r="F23" s="139"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="139"/>
+      <c r="A24" s="152"/>
       <c r="B24" s="68" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C24" s="69">
         <v>5.38402544073283E-2</v>
@@ -47779,12 +47787,12 @@
       <c r="D24" s="70">
         <v>2.6014975474054101</v>
       </c>
-      <c r="E24" s="151"/>
-      <c r="F24" s="170"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="139"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="90" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B25" s="91">
         <v>100</v>
@@ -47802,10 +47810,10 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="120" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B26" s="134" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C26" s="122">
         <v>0.204857357893384</v>
@@ -47817,15 +47825,15 @@
         <v>326</v>
       </c>
       <c r="F26" s="98" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="83" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B27" s="84" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C27" s="85">
         <v>-0.14093733148086199</v>
@@ -47840,7 +47848,7 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="124" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B28" s="125">
         <v>100</v>
@@ -47855,12 +47863,12 @@
         <v>326</v>
       </c>
       <c r="F28" s="97" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="120" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B29" s="121">
         <v>100</v>
@@ -47875,15 +47883,15 @@
         <v>326</v>
       </c>
       <c r="F29" s="97" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="86" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B30" s="87" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C30" s="88">
         <v>6.4521514360412494E-2</v>
@@ -47898,10 +47906,10 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="76" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B31" s="89" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C31" s="77">
         <v>2.36465648743483E-2</v>
@@ -47916,7 +47924,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="51" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B32" s="52">
         <v>100</v>
@@ -47934,10 +47942,10 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="90" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C33" s="92">
         <v>1.19721945732916E-2</v>
@@ -47952,10 +47960,10 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="51" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B34" s="82" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C34" s="53">
         <v>-2.4514926757940601E-4</v>
@@ -47967,12 +47975,12 @@
         <v>326</v>
       </c>
       <c r="F34" s="98" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="120" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B35" s="121">
         <v>100</v>
@@ -47987,15 +47995,15 @@
         <v>326</v>
       </c>
       <c r="F35" s="97" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="93" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B36" s="94" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C36" s="95">
         <v>-9.9338640216688701E-2</v>
@@ -48010,10 +48018,10 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="51" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B37" s="82" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C37" s="53">
         <v>8.1780585302742098E-2</v>
@@ -48025,15 +48033,15 @@
         <v>327</v>
       </c>
       <c r="F37" s="98" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="83" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B38" s="84" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C38" s="85">
         <v>-8.0581676791333205E-3</v>
@@ -48047,11 +48055,11 @@
       <c r="F38" s="98"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="140" t="s">
-        <v>493</v>
+      <c r="A39" s="153" t="s">
+        <v>492</v>
       </c>
       <c r="B39" s="66" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C39" s="55">
         <v>0.11314757691313</v>
@@ -48059,15 +48067,15 @@
       <c r="D39" s="67">
         <v>5.2656480574054196</v>
       </c>
-      <c r="E39" s="150" t="s">
+      <c r="E39" s="163" t="s">
         <v>327</v>
       </c>
-      <c r="F39" s="170"/>
+      <c r="F39" s="139"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="141"/>
+      <c r="A40" s="154"/>
       <c r="B40" s="96" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C40" s="74">
         <v>-0.116880126830938</v>
@@ -48075,15 +48083,15 @@
       <c r="D40" s="107">
         <v>2.3158929874053902</v>
       </c>
-      <c r="E40" s="151"/>
-      <c r="F40" s="170"/>
+      <c r="E40" s="164"/>
+      <c r="F40" s="139"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="76" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B41" s="89" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C41" s="77">
         <v>8.3487218640498795E-2</v>
@@ -48098,22 +48106,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="E2:E3"/>
@@ -48130,8 +48122,490 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE504C2-276F-4DD2-8CA4-71E542FA2032}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="171" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="171" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="171" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" style="172" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="172" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="171"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="171" t="s">
+        <v>615</v>
+      </c>
+      <c r="B1" s="171" t="s">
+        <v>616</v>
+      </c>
+      <c r="C1" s="171" t="s">
+        <v>619</v>
+      </c>
+      <c r="D1" s="172" t="s">
+        <v>617</v>
+      </c>
+      <c r="E1" s="172" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="171" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="172">
+        <v>-2.05993110717329</v>
+      </c>
+      <c r="C2" s="172">
+        <v>3.03645521740544</v>
+      </c>
+      <c r="D2" s="172">
+        <v>3.3904109706261301E-2</v>
+      </c>
+      <c r="E2" s="172">
+        <v>3.0308439874054298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="172">
+        <v>-2.0627486946581599</v>
+      </c>
+      <c r="C3" s="172">
+        <v>3.14684491740543</v>
+      </c>
+      <c r="D3" s="172">
+        <v>0.269542600903181</v>
+      </c>
+      <c r="E3" s="173">
+        <v>-1.12009968259455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="171" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="172">
+        <v>-0.28635675849167702</v>
+      </c>
+      <c r="C4" s="172">
+        <v>1.9749163874054401</v>
+      </c>
+      <c r="D4" s="172">
+        <v>0.244539410765303</v>
+      </c>
+      <c r="E4" s="172">
+        <v>-3.8362542594540999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="171" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="172">
+        <v>0.15461536781290999</v>
+      </c>
+      <c r="C5" s="172">
+        <v>3.88271770740544</v>
+      </c>
+      <c r="D5" s="172">
+        <v>0.15876409968765501</v>
+      </c>
+      <c r="E5" s="173">
+        <v>-0.54624473259457296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="171" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="172">
+        <v>-0.61862350960994095</v>
+      </c>
+      <c r="C6" s="172">
+        <v>3.3027707674054301</v>
+      </c>
+      <c r="D6" s="172">
+        <v>0.37717382066015598</v>
+      </c>
+      <c r="E6" s="172">
+        <v>-3.2670075425946798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="171" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="172">
+        <v>-0.48480478238550301</v>
+      </c>
+      <c r="C7" s="172">
+        <v>3.0595893874054201</v>
+      </c>
+      <c r="D7" s="172">
+        <v>0.15602959110056999</v>
+      </c>
+      <c r="E7" s="172">
+        <v>1.6800129474054299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="171" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="172">
+        <v>0.10335720262114099</v>
+      </c>
+      <c r="C8" s="172">
+        <v>4.3747270074054398</v>
+      </c>
+      <c r="D8" s="172">
+        <v>-6.5601907175453396E-3</v>
+      </c>
+      <c r="E8" s="173">
+        <v>2.5016611374053901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="171" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="172">
+        <v>-2.4285330681078698</v>
+      </c>
+      <c r="C9" s="172">
+        <v>3.0922237174054299</v>
+      </c>
+      <c r="D9" s="172">
+        <v>0.124803014354723</v>
+      </c>
+      <c r="E9" s="173">
+        <v>2.7846094374053698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="171" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="172">
+        <v>-2.6646097334453098</v>
+      </c>
+      <c r="C10" s="172" t="s">
+        <v>304</v>
+      </c>
+      <c r="D10" s="172">
+        <v>0.108073993148637</v>
+      </c>
+      <c r="E10" s="173">
+        <v>2.1188442974054098</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="171" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="172">
+        <v>-1.57324684073997</v>
+      </c>
+      <c r="C11" s="172">
+        <v>2.1743416374054001</v>
+      </c>
+      <c r="D11" s="172">
+        <v>0.42132970300595002</v>
+      </c>
+      <c r="E11" s="172">
+        <v>-0.30614277259456901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="171" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="172">
+        <v>-1.56785432271928</v>
+      </c>
+      <c r="C12" s="172">
+        <v>2.6897796274054402</v>
+      </c>
+      <c r="D12" s="172">
+        <v>0.14058912840377499</v>
+      </c>
+      <c r="E12" s="172">
+        <v>1.51702027740543</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="171" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="172">
+        <v>-1.6086314186572299</v>
+      </c>
+      <c r="C13" s="172">
+        <v>4.7865577574054399</v>
+      </c>
+      <c r="D13" s="172">
+        <v>8.9729637784239993E-2</v>
+      </c>
+      <c r="E13" s="172">
+        <v>4.4432239374053699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="171" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="172">
+        <v>-0.75224628676349903</v>
+      </c>
+      <c r="C14" s="172">
+        <v>4.8136223274054499</v>
+      </c>
+      <c r="D14" s="172">
+        <v>0.204857357893384</v>
+      </c>
+      <c r="E14" s="172">
+        <v>3.54274209740549</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="171" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="172">
+        <v>-0.94435939114414502</v>
+      </c>
+      <c r="C15" s="172">
+        <v>3.05283259740545</v>
+      </c>
+      <c r="D15" s="172">
+        <v>-0.14093733148086199</v>
+      </c>
+      <c r="E15" s="172">
+        <v>2.7234189674054501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="171" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="172">
+        <v>-2.2679323080990801</v>
+      </c>
+      <c r="C16" s="172">
+        <v>3.2920384774054399</v>
+      </c>
+      <c r="D16" s="172">
+        <v>6.4521514360412494E-2</v>
+      </c>
+      <c r="E16" s="172">
+        <v>1.5824281774054001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="172">
+        <v>-2.0928295573006701</v>
+      </c>
+      <c r="C17" s="172">
+        <v>2.3068136074054402</v>
+      </c>
+      <c r="D17" s="172">
+        <v>2.36465648743483E-2</v>
+      </c>
+      <c r="E17" s="172">
+        <v>-1.0979680625945301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="171" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="172">
+        <v>-2.5560708781736401</v>
+      </c>
+      <c r="C18" s="172">
+        <v>3.4109907274054398</v>
+      </c>
+      <c r="D18" s="172">
+        <v>4.4790606214817202E-2</v>
+      </c>
+      <c r="E18" s="172">
+        <v>2.5795764374054202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="171" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="172">
+        <v>-2.5884871133272802</v>
+      </c>
+      <c r="C19" s="172">
+        <v>3.23383048740543</v>
+      </c>
+      <c r="D19" s="172">
+        <v>1.19721945732916E-2</v>
+      </c>
+      <c r="E19" s="172">
+        <v>2.33145475740548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="171" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="172">
+        <v>-2.4742622903663598</v>
+      </c>
+      <c r="C20" s="172">
+        <v>3.23532651740544</v>
+      </c>
+      <c r="D20" s="172">
+        <v>-2.4514926757940601E-4</v>
+      </c>
+      <c r="E20" s="172">
+        <v>3.69205014740538</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="171" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="172">
+        <v>-1.567924493342</v>
+      </c>
+      <c r="C21" s="172">
+        <v>2.70142826740544</v>
+      </c>
+      <c r="D21" s="172">
+        <v>6.1160966190277897E-3</v>
+      </c>
+      <c r="E21" s="172">
+        <v>1.9454189574054199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="171" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" s="172">
+        <v>-1.8896498142260001</v>
+      </c>
+      <c r="C22" s="172">
+        <v>1.3789851174054399</v>
+      </c>
+      <c r="D22" s="172">
+        <v>-9.9338640216688701E-2</v>
+      </c>
+      <c r="E22" s="172">
+        <v>1.6440883274053699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="171" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="172">
+        <v>-2.3167328341362801</v>
+      </c>
+      <c r="C23" s="172">
+        <v>4.6105982474054397</v>
+      </c>
+      <c r="D23" s="172">
+        <v>8.1780585302742098E-2</v>
+      </c>
+      <c r="E23" s="172">
+        <v>2.4371837874053801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="171" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="172">
+        <v>-1.9827880216179401</v>
+      </c>
+      <c r="C24" s="172">
+        <v>1.63996525740543</v>
+      </c>
+      <c r="D24" s="172">
+        <v>-8.0581676791333205E-3</v>
+      </c>
+      <c r="E24" s="172">
+        <v>1.99464387740545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="171" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="172">
+        <v>-7.7828179942835002E-2</v>
+      </c>
+      <c r="C25" s="172">
+        <v>5.41741480740545</v>
+      </c>
+      <c r="D25" s="172">
+        <v>-0.116880126830938</v>
+      </c>
+      <c r="E25" s="172">
+        <v>2.3158929874053902</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="171" t="s">
+        <v>220</v>
+      </c>
+      <c r="B26" s="172">
+        <v>-0.801284650347036</v>
+      </c>
+      <c r="C26" s="172">
+        <v>4.4696641674054503</v>
+      </c>
+      <c r="D26" s="172">
+        <v>8.3487218640498795E-2</v>
+      </c>
+      <c r="E26" s="172">
+        <v>4.2852767774054401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>